<commit_message>
update prototype_4a, this closes #3
</commit_message>
<xml_diff>
--- a/planning/prototype_4a.xlsx
+++ b/planning/prototype_4a.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EthienneC/Desktop/4a/planning/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A44935-5246-9D49-B307-649F9622EDAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22360" windowHeight="14240" tabRatio="990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22360" windowHeight="14240" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loc_Methods" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter_Pages" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -187,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -239,7 +253,7 @@
       <charset val="161"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +270,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -344,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -387,23 +407,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -415,8 +420,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,6 +513,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -816,14 +845,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="15.1640625" style="1" customWidth="1"/>
@@ -835,7 +864,7 @@
     <col min="8" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -858,7 +887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -884,7 +913,7 @@
         <v>1.0196113404699423</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -910,7 +939,7 @@
         <v>1.0196113404699423</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -936,7 +965,7 @@
         <v>0.46410700351241357</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -962,7 +991,7 @@
         <v>0.21728893637694804</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -988,7 +1017,7 @@
         <v>8.364352634996762E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1014,7 +1043,7 @@
         <v>1.7945346060241649E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1040,7 +1069,7 @@
         <v>4.7920430752746268E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1066,7 +1095,7 @@
         <v>7.7337511995958133E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1092,7 +1121,7 @@
         <v>9.0495367177808636E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1118,7 +1147,7 @@
         <v>0.11154042701674756</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1144,7 +1173,7 @@
         <v>0.29432951093937959</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1170,7 +1199,7 @@
         <v>0.32010508519726777</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1196,162 +1225,162 @@
         <v>1.4890255348105541</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27">
         <f>SUM(E2:E14)</f>
         <v>260.03333333333336</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="25">
         <f>SUM(F2:F14)</f>
         <v>36.419727884695909</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="28">
         <f>SUM(G2:G14)</f>
         <v>5.2350339604157359</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+      <c r="B16" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="21">
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="24">
         <f>E15/$A$14</f>
         <v>20.002564102564104</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="24">
         <f>F15/$A$14</f>
         <v>2.801517529591993</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="28">
         <f>G15/$A$14</f>
         <v>0.40269492003197971</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="19" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="16">
         <f>G15/$A$13</f>
         <v>0.43625283003464466</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="19" t="s">
+      <c r="D18" s="19"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="16">
         <f>SQRT(C18)</f>
         <v>0.66049438304549168</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-    </row>
-    <row r="20" spans="2:7">
+      <c r="D19" s="19"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="C20"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="19" t="s">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="16">
         <f>$F$16 - 2*$C$19</f>
         <v>1.4805287635010096</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="20">
         <f>EXP(C21)</f>
         <v>4.395269124478685</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="19" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="16">
         <f>$F$16-$C$19</f>
         <v>2.1410231465465013</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="20">
         <f>EXP(C22)</f>
         <v>8.5081382493892264</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="19" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="16">
         <f>$F$16</f>
         <v>2.801517529591993</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="20">
         <f>EXP(C23)</f>
         <v>16.469620953940066</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="19" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="16">
         <f>$F$16 + $C$19</f>
         <v>3.4620119126374846</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="20">
         <f>EXP(C24)</f>
         <v>31.881053929269871</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="19" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="16">
         <f>$F$16 + 2*$C$19</f>
         <v>4.1225062956829763</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="20">
         <f>EXP(C25)</f>
         <v>61.713721431934829</v>
       </c>
@@ -1367,16 +1396,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1396,14 +1425,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="21">
         <v>7</v>
       </c>
       <c r="D2" s="15">
@@ -1419,21 +1448,21 @@
         <v>0.22410462994639299</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="22">
         <v>12</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="17">
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
@@ -1442,21 +1471,21 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="22">
         <v>10</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="17">
         <f t="shared" si="1"/>
         <v>2.3025850929940459</v>
       </c>
@@ -1465,21 +1494,21 @@
         <v>1.3624016263719349E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="22">
         <v>12</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="17">
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
@@ -1488,21 +1517,21 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="22">
         <v>10</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="17">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="17">
         <f t="shared" si="1"/>
         <v>2.3025850929940459</v>
       </c>
@@ -1511,21 +1540,21 @@
         <v>1.3624016263719349E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="22">
         <v>12</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="17">
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
@@ -1534,21 +1563,21 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="22">
         <v>12</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="17">
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
@@ -1557,21 +1586,21 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="22">
         <v>12</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="17">
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
@@ -1580,21 +1609,21 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="22">
         <v>12</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="17">
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
@@ -1603,21 +1632,21 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="22">
         <v>8</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="17">
         <f t="shared" si="1"/>
         <v>2.0794415416798357</v>
       </c>
@@ -1626,21 +1655,21 @@
         <v>0.11550856670528628</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24">
+    <row r="12" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="22">
         <v>8</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="17">
         <f t="shared" si="1"/>
         <v>2.0794415416798357</v>
       </c>
@@ -1649,21 +1678,21 @@
         <v>0.11550856670528628</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24">
+    <row r="13" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="22">
         <v>8</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="17">
         <f t="shared" si="1"/>
         <v>2.0794415416798357</v>
       </c>
@@ -1672,21 +1701,21 @@
         <v>0.11550856670528628</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24">
+    <row r="14" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="22">
         <v>20</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="17">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="17">
         <f t="shared" si="1"/>
         <v>2.9957322735539909</v>
       </c>
@@ -1695,21 +1724,21 @@
         <v>0.33226603332973415</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24">
+    <row r="15" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="22">
         <v>14</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="17">
         <f t="shared" si="1"/>
         <v>2.6390573296152584</v>
       </c>
@@ -1718,21 +1747,21 @@
         <v>4.8290183477389927E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24">
+    <row r="16" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="22">
         <v>18</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="17">
         <f t="shared" si="1"/>
         <v>2.8903717578961645</v>
       </c>
@@ -1741,21 +1770,21 @@
         <v>0.22190195492324824</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="24">
+    <row r="17" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="22">
         <v>12</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="17">
         <f t="shared" si="1"/>
         <v>2.4849066497880004</v>
       </c>
@@ -1764,156 +1793,156 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="20"/>
-      <c r="B18" s="28" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
+      <c r="B18" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21">
+      <c r="C18" s="24"/>
+      <c r="D18" s="24">
         <f>SUM(D2:D17)</f>
         <v>187</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="24">
         <f>SUM(E2:E17)</f>
         <v>38.708912869664324</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="24">
         <f>SUM(F2:F17)</f>
         <v>1.2304596827677758</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="20"/>
-      <c r="B19" s="28" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24">
         <f>D18/$A$17</f>
         <v>11.6875</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="24">
         <f>E18/A17</f>
         <v>2.4193070543540203</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="24">
         <f>F18/A17</f>
         <v>7.690373017298599E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="B21" s="19" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="16">
         <f>F18/$A$16</f>
         <v>8.2030645517851719E-2</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="B22" s="19" t="s">
+      <c r="D21" s="19"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="16">
         <f>SQRT(C21)</f>
         <v>0.28640992566224327</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="D22" s="19"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="B24" s="19" t="s">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="16">
         <f>$E$19 - 2*$C$22</f>
         <v>1.8464872030295338</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="20">
         <f>EXP(C24)</f>
         <v>6.3375179612117245</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="B25" s="19" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="16">
         <f>$E$19 - $C$22</f>
         <v>2.1328971286917771</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="20">
         <f>EXP(C25)</f>
         <v>8.43928111212605</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="B26" s="19" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="16">
         <f>$E$19</f>
         <v>2.4193070543540203</v>
       </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="20">
         <f>EXP(C26)</f>
         <v>11.23806924499352</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="B27" s="19" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="16">
         <f>$E$19 + $C$22</f>
         <v>2.7057169800162635</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="20">
         <f>EXP(C27)</f>
         <v>14.965042481379408</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="B28" s="19" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="16">
         <f>$E$19 +  2*$C$22</f>
         <v>2.9921269056785067</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="20">
         <f>EXP(C28)</f>
         <v>19.928022473189479</v>
       </c>

</xml_diff>